<commit_message>
commit the separate df_pontiac
</commit_message>
<xml_diff>
--- a/dataframe_each_make_xlsx_file/df_pontiac.xlsx
+++ b/dataframe_each_make_xlsx_file/df_pontiac.xlsx
@@ -484,8 +484,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>GTA
-only</t>
+          <t>GTA only</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -947,8 +946,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>PL1 (GT
-only*)</t>
+          <t>PL1 (GT only*)</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1309,7 +1307,11 @@
           <t>Vibe</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr"/>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
       <c r="F27" t="inlineStr">
         <is>
           <t>Information not available</t>
@@ -1437,7 +1439,11 @@
           <t>Vibe</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr"/>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
       <c r="F31" t="inlineStr">
         <is>
           <t>Information not available</t>
@@ -1565,7 +1571,11 @@
           <t>Vibe</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr"/>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
       <c r="F35" t="inlineStr">
         <is>
           <t>Information not available</t>
@@ -1726,7 +1736,11 @@
           <t>Vibe</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr"/>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
       <c r="F40" t="inlineStr">
         <is>
           <t>Information not available</t>
@@ -1887,7 +1901,11 @@
           <t>Vibe</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr"/>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
       <c r="F45" t="inlineStr">
         <is>
           <t>Information not available</t>
@@ -2413,8 +2431,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Toyota
-Immobilizer</t>
+          <t>Toyota Immobilizer</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -2711,8 +2728,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Toyota
-Immobilizer</t>
+          <t>Toyota Immobilizer</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">

</xml_diff>